<commit_message>
minor doc additions to  piping and components log
</commit_message>
<xml_diff>
--- a/docs/Converse Engine Component Specifications Log.xlsx
+++ b/docs/Converse Engine Component Specifications Log.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3915F20D-54C7-974D-A66D-60C15D5DAFAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89590176-7011-8C4A-B808-54E9C126440B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{61605A87-E3DA-CD47-956F-4305B1B3EE01}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16520" xr2:uid="{61605A87-E3DA-CD47-956F-4305B1B3EE01}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="CE001" sheetId="2" r:id="rId2"/>
+    <sheet name="CE002" sheetId="3" r:id="rId3"/>
+    <sheet name="CE003" sheetId="4" r:id="rId4"/>
+    <sheet name="CE004" sheetId="5" r:id="rId5"/>
+    <sheet name="CE005" sheetId="6" r:id="rId6"/>
+    <sheet name="CE006" sheetId="7" r:id="rId7"/>
+    <sheet name="CE007" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Part Number</t>
   </si>
@@ -92,13 +98,55 @@
   </si>
   <si>
     <t>Component Casing to hold the Engine Control Unit</t>
+  </si>
+  <si>
+    <t>External Storage</t>
+  </si>
+  <si>
+    <t>Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Lithium ion Battery</t>
+  </si>
+  <si>
+    <t>Pump</t>
+  </si>
+  <si>
+    <t>Spark igniter</t>
+  </si>
+  <si>
+    <t>Thermocouple</t>
+  </si>
+  <si>
+    <t>Pressure Transducer</t>
+  </si>
+  <si>
+    <t>CE002</t>
+  </si>
+  <si>
+    <t>CE003</t>
+  </si>
+  <si>
+    <t>CE004</t>
+  </si>
+  <si>
+    <t>CE005</t>
+  </si>
+  <si>
+    <t>CE006</t>
+  </si>
+  <si>
+    <t>CE007</t>
+  </si>
+  <si>
+    <t>CE008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +186,12 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -492,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403C0E7A-05F7-7548-AC0F-F434AB83E333}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,7 +595,86 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" location="'CE001'!A1" display="'CE001'!A1" xr:uid="{21D73DE9-30B5-334B-964F-58CB482F5AF5}"/>
   </hyperlinks>
@@ -553,9 +686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2979381-DEAA-FE43-8A31-DA3508825662}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -636,4 +767,142 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8DF5B1-5FAB-2D4C-A946-F2EC58601ED8}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13AFC054-E4A4-E245-B0AB-166D4B700B80}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD0428D-B142-C440-961C-C9EBA83CA7F0}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB040814-F0EB-5044-B30E-F217E6995994}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD90586B-5BDE-1545-9A06-DBB4644751C7}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB96BF13-0158-1743-89A3-D70F03712376}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>